<commit_message>
Drybar commit by Varaprasad 1-03-2021
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/DryBar/DryBarTestData.xlsx
+++ b/src/test/resources/TestData/DryBar/DryBarTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4770835A-E0AF-409C-808C-D8FB268A30AB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{847FA963-A4E7-4E68-AA37-76E35B06C20A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20580" windowHeight="8820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20580" windowHeight="9300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="115">
   <si>
     <t>UserName</t>
   </si>
@@ -308,6 +308,9 @@
     <t>HeaderNames</t>
   </si>
   <si>
+    <t>Liquid Glass</t>
+  </si>
+  <si>
     <t>GiftCard</t>
   </si>
   <si>
@@ -323,10 +326,52 @@
     <t xml:space="preserve">TEST4TEST  </t>
   </si>
   <si>
-    <t>Hair Products,Hair Tool,Benefit,Gifts &amp; Kits,New,How-To Inspo</t>
-  </si>
-  <si>
-    <t>Liquid Glass Smoothing Shampoo</t>
+    <t>Threedigitproductname</t>
+  </si>
+  <si>
+    <t>Hai</t>
+  </si>
+  <si>
+    <t>Fourdigitproductname</t>
+  </si>
+  <si>
+    <t>Hair</t>
+  </si>
+  <si>
+    <t>Nameofproduct</t>
+  </si>
+  <si>
+    <t>Hair Products</t>
+  </si>
+  <si>
+    <t>dublicateproductname</t>
+  </si>
+  <si>
+    <t>color care</t>
+  </si>
+  <si>
+    <t>invalidname</t>
+  </si>
+  <si>
+    <t>ppp</t>
+  </si>
+  <si>
+    <t>Pname</t>
+  </si>
+  <si>
+    <t>Shampoos</t>
+  </si>
+  <si>
+    <t>Hair Products,Hair Tools,Benefits,Gifts &amp; Kits,New,How To &amp; Inspo</t>
+  </si>
+  <si>
+    <t>0123</t>
+  </si>
+  <si>
+    <t>vicksproductname</t>
+  </si>
+  <si>
+    <t>humidifiers</t>
   </si>
 </sst>
 </file>
@@ -387,7 +432,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -407,6 +452,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -688,10 +734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AU13"/>
+  <dimension ref="A1:BB13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="W3" sqref="W3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,10 +757,10 @@
     <col min="15" max="15" width="18.28515625" customWidth="1"/>
     <col min="16" max="16" width="16.140625" customWidth="1"/>
     <col min="17" max="17" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.28515625" customWidth="1"/>
+    <col min="18" max="18" width="19.140625" customWidth="1"/>
+    <col min="19" max="19" width="26.42578125" customWidth="1"/>
     <col min="20" max="20" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="61.140625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="27.28515625" customWidth="1"/>
     <col min="25" max="25" width="11.140625" bestFit="1" customWidth="1"/>
@@ -735,9 +781,16 @@
     <col min="45" max="45" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="27.28515625" customWidth="1"/>
+    <col min="49" max="49" width="24" customWidth="1"/>
+    <col min="50" max="50" width="17.5703125" customWidth="1"/>
+    <col min="51" max="51" width="21.140625" customWidth="1"/>
+    <col min="52" max="52" width="13.28515625" customWidth="1"/>
+    <col min="53" max="53" width="10.5703125" customWidth="1"/>
+    <col min="54" max="54" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:54" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>3</v>
       </c>
@@ -808,13 +861,13 @@
         <v>92</v>
       </c>
       <c r="X1" s="10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="Y1" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Z1" s="10" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AA1" s="10"/>
       <c r="AB1" s="10" t="s">
@@ -877,8 +930,29 @@
       <c r="AU1" s="10" t="s">
         <v>59</v>
       </c>
+      <c r="AV1" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="AW1" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="AX1" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="AY1" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="AZ1" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="BA1" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="BB1" s="10" t="s">
+        <v>113</v>
+      </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -907,7 +981,7 @@
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:47" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -924,10 +998,31 @@
       <c r="O3" s="1"/>
       <c r="U3" s="5"/>
       <c r="V3" t="s">
-        <v>99</v>
+        <v>93</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>100</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>102</v>
+      </c>
+      <c r="AX3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AY3" t="s">
+        <v>106</v>
+      </c>
+      <c r="AZ3" t="s">
+        <v>108</v>
+      </c>
+      <c r="BA3" t="s">
+        <v>110</v>
+      </c>
+      <c r="BB3" t="s">
+        <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -957,7 +1052,7 @@
       <c r="U4" s="5"/>
       <c r="V4" s="3"/>
     </row>
-    <row r="5" spans="1:47" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>71</v>
       </c>
@@ -995,7 +1090,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:47" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>74</v>
       </c>
@@ -1027,7 +1122,7 @@
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -1043,7 +1138,7 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>78</v>
       </c>
@@ -1086,7 +1181,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>85</v>
       </c>
@@ -1108,7 +1203,7 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>89</v>
       </c>
@@ -1139,12 +1234,12 @@
       <c r="V10" s="3"/>
       <c r="Z10" s="7"/>
     </row>
-    <row r="11" spans="1:47" s="7" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" s="7" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>91</v>
       </c>
       <c r="W11" s="7" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="Z11"/>
       <c r="AJ11" s="7" t="s">
@@ -1184,23 +1279,23 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>93</v>
-      </c>
-      <c r="X12">
-        <v>123</v>
-      </c>
-      <c r="Y12">
-        <v>123</v>
+        <v>94</v>
+      </c>
+      <c r="X12" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y12" s="11" t="s">
+        <v>112</v>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="Z13" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Drybar New System testcases
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/DryBar/DryBarTestData.xlsx
+++ b/src/test/resources/TestData/DryBar/DryBarTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B22A8FF-9BEE-457F-B02D-6F152C241D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D55C3A17-F90F-4A18-A5A5-AD9A5756A94F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="264">
   <si>
     <t>UserName</t>
   </si>
@@ -509,9 +509,6 @@
     <t>Detox dry shampoo</t>
   </si>
   <si>
-    <t>Blow dryers</t>
-  </si>
-  <si>
     <t>Wilmington</t>
   </si>
   <si>
@@ -696,9 +693,6 @@
     <t>QA.Testing@gmail.com</t>
   </si>
   <si>
-    <t>Prasad@123</t>
-  </si>
-  <si>
     <t>NewProductDetails</t>
   </si>
   <si>
@@ -799,6 +793,33 @@
   </si>
   <si>
     <t>Schofield Barracks</t>
+  </si>
+  <si>
+    <t>19073-3972</t>
+  </si>
+  <si>
+    <t>Blow dryer Brush</t>
+  </si>
+  <si>
+    <t>Product_Name</t>
+  </si>
+  <si>
+    <t>lash blow out Mascara By IT Cosmetics</t>
+  </si>
+  <si>
+    <t>15%Couponcode</t>
+  </si>
+  <si>
+    <t>Prasad&amp;123</t>
+  </si>
+  <si>
+    <t>BUNDLE</t>
+  </si>
+  <si>
+    <t>FREECouponCode</t>
+  </si>
+  <si>
+    <t>FREE</t>
   </si>
 </sst>
 </file>
@@ -1242,84 +1263,84 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CC51"/>
+  <dimension ref="A1:CC54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="R7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AA18" sqref="AA18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="32.33203125" customWidth="1"/>
-    <col min="9" max="9" width="29.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="29.44140625" customWidth="1"/>
-    <col min="11" max="12" width="28.33203125" customWidth="1"/>
+    <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="32.28515625" customWidth="1"/>
+    <col min="9" max="9" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.42578125" customWidth="1"/>
+    <col min="11" max="12" width="28.28515625" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="34.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.5546875" customWidth="1"/>
-    <col min="16" max="16" width="18.33203125" customWidth="1"/>
-    <col min="17" max="17" width="16.109375" customWidth="1"/>
-    <col min="18" max="18" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.109375" customWidth="1"/>
-    <col min="20" max="20" width="26.44140625" customWidth="1"/>
-    <col min="21" max="21" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="32.109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="61.109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="27.33203125" customWidth="1"/>
-    <col min="26" max="26" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="60.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.5703125" customWidth="1"/>
+    <col min="16" max="16" width="18.28515625" customWidth="1"/>
+    <col min="17" max="17" width="16.140625" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.140625" customWidth="1"/>
+    <col min="20" max="20" width="26.42578125" customWidth="1"/>
+    <col min="21" max="21" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="61.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="27.28515625" customWidth="1"/>
+    <col min="26" max="26" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="60.7109375" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="4" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="14.6640625" customWidth="1"/>
-    <col min="38" max="38" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="21.109375" customWidth="1"/>
-    <col min="40" max="40" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="35.44140625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="27.33203125" customWidth="1"/>
+    <col min="30" max="30" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="14.7109375" customWidth="1"/>
+    <col min="38" max="38" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="21.140625" customWidth="1"/>
+    <col min="40" max="40" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="27.28515625" customWidth="1"/>
     <col min="50" max="50" width="24" customWidth="1"/>
-    <col min="51" max="51" width="17.5546875" customWidth="1"/>
-    <col min="52" max="52" width="21.109375" customWidth="1"/>
-    <col min="53" max="53" width="13.33203125" customWidth="1"/>
-    <col min="54" max="54" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="33.44140625" customWidth="1"/>
-    <col min="56" max="57" width="29.44140625" customWidth="1"/>
+    <col min="51" max="51" width="17.5703125" customWidth="1"/>
+    <col min="52" max="52" width="21.140625" customWidth="1"/>
+    <col min="53" max="53" width="13.28515625" customWidth="1"/>
+    <col min="54" max="54" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="33.42578125" customWidth="1"/>
+    <col min="56" max="57" width="29.42578125" customWidth="1"/>
     <col min="58" max="58" width="26" customWidth="1"/>
-    <col min="59" max="59" width="47.5546875" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="65" max="66" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="102.44140625" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="39.6640625" customWidth="1"/>
-    <col min="70" max="70" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="29.44140625" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="29.88671875" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="47.5703125" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="65" max="66" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="102.42578125" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="39.7109375" customWidth="1"/>
+    <col min="70" max="70" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="77" max="77" width="18" bestFit="1" customWidth="1"/>
     <col min="78" max="78" width="20" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:81" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:81" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>3</v>
       </c>
@@ -1348,7 +1369,7 @@
         <v>11</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K1" s="10" t="s">
         <v>20</v>
@@ -1489,7 +1510,7 @@
         <v>106</v>
       </c>
       <c r="BE1" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="BF1" s="10" t="s">
         <v>39</v>
@@ -1498,7 +1519,7 @@
         <v>118</v>
       </c>
       <c r="BH1" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="BI1" s="10" t="s">
         <v>120</v>
@@ -1528,60 +1549,60 @@
         <v>156</v>
       </c>
       <c r="BR1" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="BS1" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="BS1" s="10" t="s">
+      <c r="BT1" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="BT1" s="10" t="s">
+      <c r="BU1" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="BU1" s="10" t="s">
+      <c r="BV1" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="BV1" s="10" t="s">
+      <c r="BW1" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="BW1" s="10" t="s">
-        <v>200</v>
-      </c>
       <c r="BX1" s="10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="BY1" s="10" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="BZ1" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="CA1" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="CB1" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="CA1" s="10" t="s">
+      <c r="CC1" s="10" t="s">
         <v>225</v>
       </c>
-      <c r="CB1" s="10" t="s">
-        <v>226</v>
-      </c>
-      <c r="CC1" s="10" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="2" spans="1:81" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>146</v>
       </c>
       <c r="D2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -1594,7 +1615,7 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:81" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:81" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>66</v>
       </c>
@@ -1612,7 +1633,7 @@
       <c r="P3" s="1"/>
       <c r="V3" s="5"/>
       <c r="W3" t="s">
-        <v>160</v>
+        <v>256</v>
       </c>
       <c r="AW3" t="s">
         <v>88</v>
@@ -1636,9 +1657,9 @@
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:81" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>257</v>
       </c>
       <c r="C4" s="1"/>
       <c r="F4" s="1"/>
@@ -1649,993 +1670,1034 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
-      <c r="N4" s="1" t="s">
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="V4" s="5"/>
+      <c r="W4" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="5" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="O4" s="9" t="s">
+      <c r="O5" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="P4" s="1">
+      <c r="P5" s="1">
         <v>2025</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="Q5" t="s">
         <v>22</v>
       </c>
-      <c r="R4">
+      <c r="R5">
         <v>123</v>
       </c>
-      <c r="V4" s="5"/>
-      <c r="W4" s="3"/>
-    </row>
-    <row r="5" spans="1:81" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="V5" s="5"/>
+      <c r="W5" s="3"/>
+    </row>
+    <row r="6" spans="1:81" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>67</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" t="s">
-        <v>240</v>
-      </c>
-      <c r="E5" t="s">
-        <v>241</v>
-      </c>
-      <c r="F5" t="s">
-        <v>219</v>
-      </c>
-      <c r="G5" t="s">
-        <v>68</v>
-      </c>
-      <c r="H5" s="19" t="s">
-        <v>250</v>
-      </c>
-      <c r="I5" s="19" t="s">
-        <v>236</v>
-      </c>
-      <c r="J5" s="21"/>
-      <c r="K5" t="s">
-        <v>176</v>
-      </c>
-      <c r="L5" s="20" t="s">
-        <v>251</v>
-      </c>
-      <c r="M5">
-        <v>8500563032</v>
-      </c>
-      <c r="Y5" s="4"/>
-      <c r="Z5" s="2"/>
-      <c r="AC5" s="3">
-        <v>123</v>
-      </c>
-      <c r="BG5" s="1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="6" spans="1:81" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>69</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" t="s">
-        <v>141</v>
+        <v>238</v>
       </c>
       <c r="E6" t="s">
-        <v>181</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>221</v>
+        <v>239</v>
+      </c>
+      <c r="F6" t="s">
+        <v>218</v>
       </c>
       <c r="G6" t="s">
         <v>68</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="I6" s="1" t="s">
+      <c r="H6" s="19" t="s">
+        <v>248</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>234</v>
+      </c>
+      <c r="J6" s="21"/>
+      <c r="K6" t="s">
+        <v>175</v>
+      </c>
+      <c r="L6" s="20" t="s">
+        <v>249</v>
+      </c>
+      <c r="M6">
+        <v>8500563032</v>
+      </c>
+      <c r="Y6" s="4"/>
+      <c r="Z6" s="2"/>
+      <c r="AC6" s="3">
+        <v>123</v>
+      </c>
+      <c r="BG6" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="7" spans="1:81" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" t="s">
+        <v>141</v>
+      </c>
+      <c r="E7" t="s">
+        <v>180</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="G7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="L6" s="1">
-        <v>15014</v>
-      </c>
-      <c r="M6" s="1">
+      <c r="I7" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="M7" s="1">
         <v>9998999999</v>
       </c>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-    </row>
-    <row r="7" spans="1:81" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+    </row>
+    <row r="8" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-    </row>
-    <row r="8" spans="1:81" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C8" t="s">
-        <v>71</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="S8" t="s">
-        <v>73</v>
-      </c>
-      <c r="T8" t="s">
-        <v>74</v>
-      </c>
-      <c r="U8" t="s">
-        <v>75</v>
-      </c>
-      <c r="V8" t="s">
-        <v>76</v>
-      </c>
-      <c r="AD8" t="s">
-        <v>24</v>
-      </c>
-      <c r="AE8" t="s">
-        <v>26</v>
-      </c>
-      <c r="AF8">
-        <v>123456</v>
-      </c>
-      <c r="AG8" t="s">
-        <v>29</v>
-      </c>
-      <c r="AH8" t="s">
-        <v>31</v>
-      </c>
-      <c r="AI8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:81" x14ac:dyDescent="0.3">
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>77</v>
-      </c>
-      <c r="B9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>8</v>
+        <v>70</v>
+      </c>
+      <c r="C9" t="s">
+        <v>71</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>2</v>
+        <v>72</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:81" x14ac:dyDescent="0.3">
+      <c r="S9" t="s">
+        <v>73</v>
+      </c>
+      <c r="T9" t="s">
+        <v>74</v>
+      </c>
+      <c r="U9" t="s">
+        <v>75</v>
+      </c>
+      <c r="V9" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF9">
+        <v>123456</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="F10" s="1"/>
+        <v>77</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1" t="s">
+    </row>
+    <row r="11" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="O10" s="9" t="s">
+      <c r="O11" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="P10" s="1">
+      <c r="P11" s="1">
         <v>2025</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="Q11" t="s">
         <v>22</v>
       </c>
-      <c r="R10">
+      <c r="R11">
         <v>123</v>
       </c>
-      <c r="V10" s="5"/>
-      <c r="W10" s="3"/>
-      <c r="AA10" s="7"/>
-    </row>
-    <row r="11" spans="1:81" s="7" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
+      <c r="V11" s="5"/>
+      <c r="W11" s="3"/>
+      <c r="AA11" s="7"/>
+    </row>
+    <row r="12" spans="1:81" s="7" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="X11" s="7" t="s">
+      <c r="X12" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="AA11"/>
-      <c r="AK11" s="7" t="s">
+      <c r="AA12"/>
+      <c r="AK12" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="AL11" s="7" t="s">
+      <c r="AL12" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="AM11" s="8" t="s">
+      <c r="AM12" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="AN11" s="7" t="s">
+      <c r="AN12" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AO11" s="7" t="s">
+      <c r="AO12" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="AP11" s="7" t="s">
+      <c r="AP12" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="AQ11" s="7">
+      <c r="AQ12" s="7">
         <v>27</v>
       </c>
-      <c r="AR11" s="7" t="s">
+      <c r="AR12" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="AS11" s="7" t="s">
+      <c r="AS12" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="AT11" s="7" t="s">
+      <c r="AT12" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="AU11" s="7">
+      <c r="AU12" s="7">
         <v>2</v>
       </c>
-      <c r="AV11" s="7" t="s">
+      <c r="AV12" s="7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:81" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="13" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>83</v>
       </c>
-      <c r="Y12" s="11" t="s">
-        <v>214</v>
-      </c>
-      <c r="Z12" s="11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="13" spans="1:81" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>193</v>
-      </c>
       <c r="Y13" s="11" t="s">
-        <v>244</v>
+        <v>213</v>
       </c>
       <c r="Z13" s="11" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>245</v>
+        <v>192</v>
       </c>
       <c r="Y14" s="11" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="Z14" s="11" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="Y15" s="11" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="Z15" s="11" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:81" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y16" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="Z16" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>262</v>
+      </c>
+      <c r="Y17" s="11"/>
+      <c r="Z17" s="11"/>
+      <c r="AA17" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="18" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>259</v>
+      </c>
+      <c r="Y18" s="11"/>
+      <c r="Z18" s="11"/>
+      <c r="AA18" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="19" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>86</v>
       </c>
-      <c r="AA16" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="17" spans="1:68" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="AA19" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="20" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>165</v>
+      </c>
+      <c r="AA20" t="s">
         <v>166</v>
       </c>
-      <c r="AA17" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="18" spans="1:68" ht="316.8" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    </row>
+    <row r="21" spans="1:67" ht="360" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>105</v>
       </c>
-      <c r="BD18" s="12" t="s">
-        <v>249</v>
-      </c>
-      <c r="BE18" s="12" t="s">
-        <v>217</v>
-      </c>
-      <c r="BF18" t="s">
+      <c r="BD21" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="BE21" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="BF21" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="1:68" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="22" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>108</v>
       </c>
-      <c r="N19" t="s">
+      <c r="N22" t="s">
         <v>19</v>
       </c>
-      <c r="O19" s="14" t="s">
+      <c r="O22" s="14" t="s">
         <v>78</v>
-      </c>
-      <c r="P19" s="2">
-        <v>2025</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>22</v>
-      </c>
-      <c r="R19" s="3">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="20" spans="1:68" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="N20" t="s">
-        <v>103</v>
-      </c>
-      <c r="O20" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="P20" s="2">
-        <v>2025</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>111</v>
-      </c>
-      <c r="R20" s="3">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="21" spans="1:68" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="N21" t="s">
-        <v>102</v>
-      </c>
-      <c r="O21" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="P21" s="2">
-        <v>2025</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>112</v>
-      </c>
-      <c r="R21" s="3">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="22" spans="1:68" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>114</v>
-      </c>
-      <c r="N22" t="s">
-        <v>101</v>
-      </c>
-      <c r="O22" s="11" t="s">
-        <v>117</v>
       </c>
       <c r="P22" s="2">
         <v>2025</v>
       </c>
       <c r="Q22" t="s">
-        <v>111</v>
+        <v>22</v>
       </c>
       <c r="R22" s="3">
         <v>123</v>
       </c>
     </row>
-    <row r="23" spans="1:68" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+    <row r="23" spans="1:67" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="N23" t="s">
+        <v>103</v>
+      </c>
+      <c r="O23" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="P23" s="2">
+        <v>2025</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>111</v>
+      </c>
+      <c r="R23" s="3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" spans="1:67" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="N24" t="s">
+        <v>102</v>
+      </c>
+      <c r="O24" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="P24" s="2">
+        <v>2025</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>112</v>
+      </c>
+      <c r="R24" s="3">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="25" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>114</v>
+      </c>
+      <c r="N25" t="s">
+        <v>101</v>
+      </c>
+      <c r="O25" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="P25" s="2">
+        <v>2025</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>111</v>
+      </c>
+      <c r="R25" s="3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>119</v>
       </c>
-      <c r="O23" s="11"/>
-      <c r="BH23" t="s">
-        <v>220</v>
-      </c>
-      <c r="BI23" t="s">
+      <c r="O26" s="11"/>
+      <c r="BH26" t="s">
+        <v>219</v>
+      </c>
+      <c r="BI26" t="s">
         <v>120</v>
       </c>
-      <c r="BJ23" t="s">
+      <c r="BJ26" t="s">
         <v>121</v>
       </c>
-      <c r="BK23" t="s">
+      <c r="BK26" t="s">
         <v>122</v>
       </c>
-      <c r="BL23" t="s">
+      <c r="BL26" t="s">
         <v>123</v>
       </c>
-      <c r="BM23" t="s">
+      <c r="BM26" t="s">
         <v>126</v>
       </c>
-      <c r="BN23" t="s">
+      <c r="BN26" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="24" spans="1:68" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="27" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>128</v>
       </c>
-      <c r="BO24" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="25" spans="1:68" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="BO27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="28" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>131</v>
       </c>
-      <c r="BO25" t="s">
+      <c r="BO28" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="26" spans="1:68" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="29" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>132</v>
       </c>
-      <c r="BO26" t="s">
+      <c r="BO29" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="27" spans="1:68" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+    <row r="30" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>134</v>
       </c>
-      <c r="BO27" t="s">
+      <c r="BO30" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="31" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>135</v>
+      </c>
+      <c r="BO31" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="32" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>137</v>
+      </c>
+      <c r="BO32" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="33" spans="1:76" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>139</v>
+      </c>
+      <c r="D33" t="s">
+        <v>141</v>
+      </c>
+      <c r="E33" t="s">
+        <v>180</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="BP33" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="34" spans="1:76" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>144</v>
+      </c>
+      <c r="B34" t="s">
+        <v>145</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="35" spans="1:76" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>147</v>
+      </c>
+      <c r="BO35" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="36" spans="1:76" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>150</v>
+      </c>
+      <c r="BO36" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="37" spans="1:76" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>152</v>
+      </c>
+      <c r="BO37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="38" spans="1:76" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>153</v>
+      </c>
+      <c r="AB38" s="17" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="39" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>172</v>
+      </c>
+      <c r="BQ39" s="18" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="40" spans="1:76" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>231</v>
+      </c>
+      <c r="C40" s="1"/>
+      <c r="D40" t="s">
+        <v>191</v>
+      </c>
+      <c r="E40" t="s">
+        <v>8</v>
+      </c>
+      <c r="F40" s="1" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="28" spans="1:68" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>135</v>
-      </c>
-      <c r="BO28" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="29" spans="1:68" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>137</v>
-      </c>
-      <c r="BO29" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="30" spans="1:68" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>139</v>
-      </c>
-      <c r="D30" t="s">
-        <v>141</v>
-      </c>
-      <c r="E30" t="s">
-        <v>181</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="BP30" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="31" spans="1:68" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>144</v>
-      </c>
-      <c r="B31" t="s">
-        <v>145</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="32" spans="1:68" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>147</v>
-      </c>
-      <c r="BO32" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="33" spans="1:76" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>150</v>
-      </c>
-      <c r="BO33" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="34" spans="1:76" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>152</v>
-      </c>
-      <c r="BO34" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="35" spans="1:76" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>153</v>
-      </c>
-      <c r="AB35" s="17" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="36" spans="1:76" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>173</v>
-      </c>
-      <c r="BQ36" s="18" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="37" spans="1:76" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>233</v>
-      </c>
-      <c r="C37" s="1"/>
-      <c r="D37" t="s">
-        <v>192</v>
-      </c>
-      <c r="E37" t="s">
+      <c r="G40" t="s">
+        <v>68</v>
+      </c>
+      <c r="H40" t="s">
+        <v>163</v>
+      </c>
+      <c r="I40" t="s">
+        <v>160</v>
+      </c>
+      <c r="K40" t="s">
+        <v>232</v>
+      </c>
+      <c r="L40">
+        <v>72729</v>
+      </c>
+      <c r="M40" s="11" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="41" spans="1:76" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>158</v>
+      </c>
+      <c r="W41" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="42" spans="1:76" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>164</v>
+      </c>
+      <c r="C42" s="1"/>
+      <c r="D42" t="s">
+        <v>191</v>
+      </c>
+      <c r="E42" t="s">
         <v>8</v>
       </c>
-      <c r="F37" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="G37" t="s">
-        <v>68</v>
-      </c>
-      <c r="H37" t="s">
-        <v>164</v>
-      </c>
-      <c r="I37" t="s">
-        <v>161</v>
-      </c>
-      <c r="K37" t="s">
-        <v>234</v>
-      </c>
-      <c r="L37">
-        <v>72729</v>
-      </c>
-      <c r="M37" s="11" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="38" spans="1:76" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>158</v>
-      </c>
-      <c r="W38" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="39" spans="1:76" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>165</v>
-      </c>
-      <c r="C39" s="1"/>
-      <c r="D39" t="s">
-        <v>192</v>
-      </c>
-      <c r="E39" t="s">
-        <v>8</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="G39" t="s">
-        <v>68</v>
-      </c>
-      <c r="H39" t="s">
-        <v>164</v>
-      </c>
-      <c r="I39" t="s">
-        <v>161</v>
-      </c>
-      <c r="K39" t="s">
-        <v>162</v>
-      </c>
-      <c r="L39">
-        <v>19702</v>
-      </c>
-      <c r="M39" s="11" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="40" spans="1:76" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>182</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="41" spans="1:76" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>168</v>
-      </c>
-      <c r="W41" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="42" spans="1:76" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>170</v>
-      </c>
-      <c r="D42" t="s">
-        <v>188</v>
-      </c>
-      <c r="E42" t="s">
-        <v>191</v>
-      </c>
       <c r="F42" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G42" t="s">
         <v>68</v>
       </c>
       <c r="H42" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="I42" t="s">
-        <v>253</v>
+        <v>160</v>
       </c>
       <c r="K42" t="s">
-        <v>252</v>
-      </c>
-      <c r="L42" s="11">
-        <v>74058</v>
+        <v>161</v>
+      </c>
+      <c r="L42">
+        <v>19702</v>
       </c>
       <c r="M42" s="11" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="43" spans="1:76" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="43" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>179</v>
-      </c>
-      <c r="C43" s="1"/>
-      <c r="D43" t="s">
-        <v>189</v>
-      </c>
-      <c r="E43" t="s">
+        <v>181</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="44" spans="1:76" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>167</v>
+      </c>
+      <c r="W44" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="45" spans="1:76" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>169</v>
+      </c>
+      <c r="D45" t="s">
+        <v>187</v>
+      </c>
+      <c r="E45" t="s">
         <v>190</v>
       </c>
-      <c r="F43" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="G43" t="s">
-        <v>68</v>
-      </c>
-      <c r="H43" s="22" t="s">
-        <v>184</v>
-      </c>
-      <c r="I43" s="19" t="s">
-        <v>185</v>
-      </c>
-      <c r="J43" s="19" t="s">
-        <v>180</v>
-      </c>
-      <c r="K43" t="s">
-        <v>186</v>
-      </c>
-      <c r="L43" s="20" t="s">
-        <v>242</v>
-      </c>
-      <c r="M43" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="Y43" s="4"/>
-      <c r="Z43" s="2"/>
-      <c r="AC43" s="3">
-        <v>123</v>
-      </c>
-      <c r="BG43" s="1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="44" spans="1:76" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>194</v>
-      </c>
-      <c r="BR44">
-        <v>399</v>
-      </c>
-      <c r="BS44" t="s">
-        <v>141</v>
-      </c>
-      <c r="BT44" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="BU44" t="s">
-        <v>201</v>
-      </c>
-      <c r="BV44" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="BW44" t="s">
-        <v>203</v>
-      </c>
-      <c r="BX44" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="45" spans="1:76" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>205</v>
-      </c>
-      <c r="D45" t="s">
-        <v>188</v>
-      </c>
-      <c r="E45" t="s">
-        <v>191</v>
-      </c>
       <c r="F45" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G45" t="s">
         <v>68</v>
       </c>
       <c r="H45" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I45" t="s">
-        <v>172</v>
+        <v>251</v>
       </c>
       <c r="K45" t="s">
-        <v>206</v>
+        <v>250</v>
       </c>
       <c r="L45" s="11">
         <v>74058</v>
       </c>
       <c r="M45" s="11" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="46" spans="1:76" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="46" spans="1:76" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>207</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="C46" s="1"/>
       <c r="D46" t="s">
         <v>188</v>
       </c>
       <c r="E46" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G46" t="s">
         <v>68</v>
       </c>
-      <c r="H46" t="s">
-        <v>171</v>
-      </c>
-      <c r="I46" t="s">
-        <v>172</v>
+      <c r="H46" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="I46" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="J46" s="19" t="s">
+        <v>179</v>
       </c>
       <c r="K46" t="s">
-        <v>208</v>
-      </c>
-      <c r="L46" s="11">
-        <v>74058</v>
+        <v>185</v>
+      </c>
+      <c r="L46" s="20" t="s">
+        <v>240</v>
       </c>
       <c r="M46" s="11" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="47" spans="1:76" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+      <c r="Y46" s="4"/>
+      <c r="Z46" s="2"/>
+      <c r="AC46" s="3">
+        <v>123</v>
+      </c>
+      <c r="BG46" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="47" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>209</v>
-      </c>
-      <c r="D47" t="s">
-        <v>188</v>
-      </c>
-      <c r="E47" t="s">
-        <v>191</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="G47" t="s">
-        <v>68</v>
-      </c>
-      <c r="H47" t="s">
-        <v>171</v>
-      </c>
-      <c r="I47" t="s">
-        <v>172</v>
-      </c>
-      <c r="K47" t="s">
-        <v>210</v>
-      </c>
-      <c r="L47" s="11">
-        <v>74058</v>
-      </c>
-      <c r="M47" s="11" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="48" spans="1:76" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+      <c r="BR47">
+        <v>399</v>
+      </c>
+      <c r="BS47" t="s">
+        <v>141</v>
+      </c>
+      <c r="BT47" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="BU47" t="s">
+        <v>200</v>
+      </c>
+      <c r="BV47" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="BW47" t="s">
+        <v>202</v>
+      </c>
+      <c r="BX47" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="48" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>211</v>
-      </c>
-      <c r="C48" s="1"/>
+        <v>204</v>
+      </c>
       <c r="D48" t="s">
-        <v>7</v>
+        <v>187</v>
       </c>
       <c r="E48" t="s">
-        <v>8</v>
-      </c>
-      <c r="F48" t="s">
-        <v>219</v>
+        <v>190</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>218</v>
       </c>
       <c r="G48" t="s">
         <v>68</v>
       </c>
-      <c r="H48" s="19" t="s">
-        <v>174</v>
-      </c>
-      <c r="I48" s="19" t="s">
-        <v>254</v>
-      </c>
-      <c r="J48" s="21"/>
+      <c r="H48" t="s">
+        <v>170</v>
+      </c>
+      <c r="I48" t="s">
+        <v>171</v>
+      </c>
       <c r="K48" t="s">
+        <v>205</v>
+      </c>
+      <c r="L48" s="11">
+        <v>74058</v>
+      </c>
+      <c r="M48" s="11" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="49" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>206</v>
       </c>
-      <c r="L48" s="20">
-        <v>99702</v>
-      </c>
-      <c r="M48">
-        <v>8500563032</v>
-      </c>
-      <c r="Y48" s="4"/>
-      <c r="Z48" s="2"/>
-      <c r="AC48" s="3">
-        <v>123</v>
-      </c>
-      <c r="BG48" s="1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="49" spans="1:81" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>212</v>
-      </c>
-      <c r="C49" s="1"/>
       <c r="D49" t="s">
-        <v>7</v>
+        <v>187</v>
       </c>
       <c r="E49" t="s">
-        <v>8</v>
-      </c>
-      <c r="F49" t="s">
-        <v>219</v>
+        <v>190</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>218</v>
       </c>
       <c r="G49" t="s">
         <v>68</v>
       </c>
-      <c r="H49" s="19" t="s">
-        <v>255</v>
-      </c>
-      <c r="I49" s="19" t="s">
-        <v>256</v>
-      </c>
-      <c r="J49" s="21"/>
+      <c r="H49" t="s">
+        <v>170</v>
+      </c>
+      <c r="I49" t="s">
+        <v>171</v>
+      </c>
       <c r="K49" t="s">
+        <v>207</v>
+      </c>
+      <c r="L49" s="11">
+        <v>74058</v>
+      </c>
+      <c r="M49" s="11" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="50" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>208</v>
       </c>
-      <c r="L49" s="20">
-        <v>96857</v>
-      </c>
-      <c r="M49">
-        <v>8500563032</v>
-      </c>
-      <c r="Y49" s="4"/>
-      <c r="Z49" s="2"/>
-      <c r="AC49" s="3">
-        <v>123</v>
-      </c>
-      <c r="BG49" s="1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="50" spans="1:81" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>213</v>
-      </c>
-      <c r="C50" s="1"/>
       <c r="D50" t="s">
-        <v>7</v>
+        <v>187</v>
       </c>
       <c r="E50" t="s">
-        <v>8</v>
+        <v>190</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G50" t="s">
         <v>68</v>
       </c>
-      <c r="H50" s="19" t="s">
+      <c r="H50" t="s">
+        <v>170</v>
+      </c>
+      <c r="I50" t="s">
+        <v>171</v>
+      </c>
+      <c r="K50" t="s">
+        <v>209</v>
+      </c>
+      <c r="L50" s="11">
+        <v>74058</v>
+      </c>
+      <c r="M50" s="11" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="51" spans="1:81" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>210</v>
+      </c>
+      <c r="C51" s="1"/>
+      <c r="D51" t="s">
+        <v>7</v>
+      </c>
+      <c r="E51" t="s">
+        <v>8</v>
+      </c>
+      <c r="F51" t="s">
+        <v>218</v>
+      </c>
+      <c r="G51" t="s">
+        <v>68</v>
+      </c>
+      <c r="H51" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="I51" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="J51" s="21"/>
+      <c r="K51" t="s">
+        <v>205</v>
+      </c>
+      <c r="L51" s="20">
+        <v>99702</v>
+      </c>
+      <c r="M51">
+        <v>8500563032</v>
+      </c>
+      <c r="Y51" s="4"/>
+      <c r="Z51" s="2"/>
+      <c r="AC51" s="3">
+        <v>123</v>
+      </c>
+      <c r="BG51" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="52" spans="1:81" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>211</v>
+      </c>
+      <c r="C52" s="1"/>
+      <c r="D52" t="s">
+        <v>7</v>
+      </c>
+      <c r="E52" t="s">
+        <v>8</v>
+      </c>
+      <c r="F52" t="s">
+        <v>218</v>
+      </c>
+      <c r="G52" t="s">
+        <v>68</v>
+      </c>
+      <c r="H52" s="19" t="s">
+        <v>253</v>
+      </c>
+      <c r="I52" s="19" t="s">
+        <v>254</v>
+      </c>
+      <c r="J52" s="21"/>
+      <c r="K52" t="s">
+        <v>207</v>
+      </c>
+      <c r="L52" s="20">
+        <v>96857</v>
+      </c>
+      <c r="M52">
+        <v>8500563032</v>
+      </c>
+      <c r="Y52" s="4"/>
+      <c r="Z52" s="2"/>
+      <c r="AC52" s="3">
+        <v>123</v>
+      </c>
+      <c r="BG52" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="53" spans="1:81" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>212</v>
+      </c>
+      <c r="C53" s="1"/>
+      <c r="D53" t="s">
+        <v>7</v>
+      </c>
+      <c r="E53" t="s">
+        <v>8</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="G53" t="s">
+        <v>68</v>
+      </c>
+      <c r="H53" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="I53" s="19" t="s">
         <v>174</v>
       </c>
-      <c r="I50" s="19" t="s">
-        <v>175</v>
-      </c>
-      <c r="J50" s="21"/>
-      <c r="K50" t="s">
-        <v>210</v>
-      </c>
-      <c r="L50" s="20">
+      <c r="J53" s="21"/>
+      <c r="K53" t="s">
+        <v>209</v>
+      </c>
+      <c r="L53" s="20">
         <v>75163</v>
       </c>
-      <c r="M50">
+      <c r="M53">
         <v>8500563032</v>
       </c>
-      <c r="Y50" s="4"/>
-      <c r="Z50" s="2"/>
-      <c r="AC50" s="3">
+      <c r="Y53" s="4"/>
+      <c r="Z53" s="2"/>
+      <c r="AC53" s="3">
         <v>123</v>
       </c>
-      <c r="BG50" s="1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="51" spans="1:81" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>223</v>
-      </c>
-      <c r="BY51" t="s">
+      <c r="BG53" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="54" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>221</v>
+      </c>
+      <c r="BY54" t="s">
+        <v>228</v>
+      </c>
+      <c r="BZ54" t="s">
+        <v>227</v>
+      </c>
+      <c r="CA54" s="23" t="s">
         <v>230</v>
       </c>
-      <c r="BZ51" t="s">
-        <v>229</v>
-      </c>
-      <c r="CA51" s="23" t="s">
-        <v>232</v>
-      </c>
-      <c r="CB51" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="CC51">
+      <c r="CB54" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="CC54">
         <v>100</v>
       </c>
     </row>
@@ -2643,27 +2705,27 @@
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{0EE2B951-04E0-4C37-AD27-41ABE90F13C8}"/>
     <hyperlink ref="C2" r:id="rId2" display="drybar@123" xr:uid="{1E2EF8D6-0728-4603-8801-14D9C148AAC7}"/>
-    <hyperlink ref="BG5" r:id="rId3" xr:uid="{7EAA2625-5DF5-4A43-BFD0-B64018446D5D}"/>
-    <hyperlink ref="F30" r:id="rId4" xr:uid="{85702DA2-6B99-4F4A-9AA2-9F1D91BC8E3A}"/>
-    <hyperlink ref="F40" r:id="rId5" xr:uid="{40C27E8C-3B81-4D20-A6BC-3DB1743540AE}"/>
-    <hyperlink ref="C40" r:id="rId6" display="drybar@1234" xr:uid="{BF124FBE-91BB-4F73-8DBB-84F5B8683E1F}"/>
-    <hyperlink ref="BG43" r:id="rId7" xr:uid="{88CA8FE1-1EE7-43F7-B68C-97F732683303}"/>
-    <hyperlink ref="F43" r:id="rId8" xr:uid="{1FC1E3B9-88CF-43FC-A071-AA48E7C05E78}"/>
-    <hyperlink ref="F42" r:id="rId9" display="yoga.manoj6@gmail.com" xr:uid="{115A8F90-5F25-49F7-B091-7E933F782B63}"/>
-    <hyperlink ref="BT44" r:id="rId10" xr:uid="{D521859E-FD3C-4036-902B-011CAFF82DC1}"/>
-    <hyperlink ref="BV44" r:id="rId11" xr:uid="{3CF69B76-2A0C-4F79-A3E3-ED222697DC52}"/>
-    <hyperlink ref="F45" r:id="rId12" display="yoga.manoj6@gmail.com" xr:uid="{9A1EC28A-A256-4B40-B2C7-1472DDDDFA8A}"/>
-    <hyperlink ref="F46" r:id="rId13" display="yoga.manoj6@gmail.com" xr:uid="{61095286-9BF8-473F-9D28-6346EED8AE04}"/>
-    <hyperlink ref="F47" r:id="rId14" display="yoga.manoj6@gmail.com" xr:uid="{B45D2FAE-E215-4BE1-9874-E325BAF9C7F4}"/>
-    <hyperlink ref="BG48" r:id="rId15" xr:uid="{14C25E77-F645-4DDA-8E89-5F05454FA784}"/>
-    <hyperlink ref="BG49" r:id="rId16" xr:uid="{6A156A81-D2AB-481C-AE1E-982B2AFF941D}"/>
-    <hyperlink ref="BG50" r:id="rId17" xr:uid="{6FF3B2A5-29F8-4063-8E70-87A8855AC718}"/>
-    <hyperlink ref="F39" r:id="rId18" xr:uid="{81F356DF-5BE2-4BA2-8CF2-EA86237D44D0}"/>
-    <hyperlink ref="F50" r:id="rId19" display="raikanti.prasad906@gmail.coma.manoj6@gmail.com" xr:uid="{3350012F-B83F-4459-920D-B43C2D9B639D}"/>
+    <hyperlink ref="BG6" r:id="rId3" xr:uid="{7EAA2625-5DF5-4A43-BFD0-B64018446D5D}"/>
+    <hyperlink ref="F33" r:id="rId4" xr:uid="{85702DA2-6B99-4F4A-9AA2-9F1D91BC8E3A}"/>
+    <hyperlink ref="F43" r:id="rId5" xr:uid="{40C27E8C-3B81-4D20-A6BC-3DB1743540AE}"/>
+    <hyperlink ref="C43" r:id="rId6" display="drybar@1234" xr:uid="{BF124FBE-91BB-4F73-8DBB-84F5B8683E1F}"/>
+    <hyperlink ref="BG46" r:id="rId7" xr:uid="{88CA8FE1-1EE7-43F7-B68C-97F732683303}"/>
+    <hyperlink ref="F46" r:id="rId8" xr:uid="{1FC1E3B9-88CF-43FC-A071-AA48E7C05E78}"/>
+    <hyperlink ref="F45" r:id="rId9" display="yoga.manoj6@gmail.com" xr:uid="{115A8F90-5F25-49F7-B091-7E933F782B63}"/>
+    <hyperlink ref="BT47" r:id="rId10" xr:uid="{D521859E-FD3C-4036-902B-011CAFF82DC1}"/>
+    <hyperlink ref="BV47" r:id="rId11" xr:uid="{3CF69B76-2A0C-4F79-A3E3-ED222697DC52}"/>
+    <hyperlink ref="F48" r:id="rId12" display="yoga.manoj6@gmail.com" xr:uid="{9A1EC28A-A256-4B40-B2C7-1472DDDDFA8A}"/>
+    <hyperlink ref="F49" r:id="rId13" display="yoga.manoj6@gmail.com" xr:uid="{61095286-9BF8-473F-9D28-6346EED8AE04}"/>
+    <hyperlink ref="F50" r:id="rId14" display="yoga.manoj6@gmail.com" xr:uid="{B45D2FAE-E215-4BE1-9874-E325BAF9C7F4}"/>
+    <hyperlink ref="BG51" r:id="rId15" xr:uid="{14C25E77-F645-4DDA-8E89-5F05454FA784}"/>
+    <hyperlink ref="BG52" r:id="rId16" xr:uid="{6A156A81-D2AB-481C-AE1E-982B2AFF941D}"/>
+    <hyperlink ref="BG53" r:id="rId17" xr:uid="{6FF3B2A5-29F8-4063-8E70-87A8855AC718}"/>
+    <hyperlink ref="F42" r:id="rId18" xr:uid="{81F356DF-5BE2-4BA2-8CF2-EA86237D44D0}"/>
+    <hyperlink ref="F53" r:id="rId19" display="raikanti.prasad906@gmail.coma.manoj6@gmail.com" xr:uid="{3350012F-B83F-4459-920D-B43C2D9B639D}"/>
     <hyperlink ref="F2" r:id="rId20" xr:uid="{8664094E-880D-411A-9CED-16762BE15860}"/>
-    <hyperlink ref="C31" r:id="rId21" xr:uid="{CBE671E4-46B4-415B-8E4C-3A352D473E9F}"/>
-    <hyperlink ref="F37" r:id="rId22" xr:uid="{C228D363-CFA1-48C1-8328-0F96697D7CBE}"/>
-    <hyperlink ref="F6" r:id="rId23" xr:uid="{483E9E5E-00DA-432B-8D87-00F6E882902B}"/>
+    <hyperlink ref="C34" r:id="rId21" display="Prasad@123" xr:uid="{CBE671E4-46B4-415B-8E4C-3A352D473E9F}"/>
+    <hyperlink ref="F40" r:id="rId22" xr:uid="{C228D363-CFA1-48C1-8328-0F96697D7CBE}"/>
+    <hyperlink ref="F7" r:id="rId23" xr:uid="{483E9E5E-00DA-432B-8D87-00F6E882902B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId24"/>

</xml_diff>